<commit_message>
1) Fine-tuned the bus coordinates of the 29-bus GB transmission network. Now the network topology has no overlapped lines and fits well with the windstorm contours.
</commit_message>
<xml_diff>
--- a/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
+++ b/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\GB_Network_29bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC8835B-29A1-47B5-A956-BB926D14AC4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F58723A-0D73-4121-97EF-293CCD09AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F290B48-A8E1-43D7-A531-2D8691AE6FE2}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -602,10 +602,10 @@
         <v>0.5</v>
       </c>
       <c r="H2">
-        <v>-3.7309283</v>
+        <v>-4.67</v>
       </c>
       <c r="I2">
-        <v>50.471673299999999</v>
+        <v>50.35</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
@@ -631,10 +631,10 @@
         <v>0.5</v>
       </c>
       <c r="H3">
-        <v>-3.1368499999999999</v>
+        <v>-1.75</v>
       </c>
       <c r="I3">
-        <v>51.203884000000002</v>
+        <v>50.1</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
@@ -660,10 +660,10 @@
         <v>0.5</v>
       </c>
       <c r="H4">
-        <v>-3.4032144</v>
+        <v>-3.32</v>
       </c>
       <c r="I4">
-        <v>51.388336600000002</v>
+        <v>50.690000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -689,10 +689,10 @@
         <v>0.5</v>
       </c>
       <c r="H5">
-        <v>-3.687792</v>
+        <v>-0.44</v>
       </c>
       <c r="I5">
-        <v>52.535903699999999</v>
+        <v>50.52</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -718,10 +718,10 @@
         <v>0.5</v>
       </c>
       <c r="H6">
-        <v>-4.1364786999999996</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>51.005904899999997</v>
+        <v>50.95</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
@@ -747,10 +747,10 @@
         <v>0.5</v>
       </c>
       <c r="H7">
-        <v>-1.0957412</v>
+        <v>-0.05</v>
       </c>
       <c r="I7">
-        <v>52.530187599999998</v>
+        <v>51.370000000000005</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
@@ -776,10 +776,10 @@
         <v>0.5</v>
       </c>
       <c r="H8">
-        <v>-2.9246376999999999</v>
+        <v>-2.0499999999999998</v>
       </c>
       <c r="I8">
-        <v>50.786499800000001</v>
+        <v>51.2</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
@@ -805,10 +805,10 @@
         <v>0.5</v>
       </c>
       <c r="H9">
-        <v>-3.8324674999999999</v>
+        <v>-4.37</v>
       </c>
       <c r="I9">
-        <v>51.316997600000001</v>
+        <v>51.67</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
@@ -834,10 +834,10 @@
         <v>0.5</v>
       </c>
       <c r="H10">
-        <v>-2.7561477999999999</v>
+        <v>-0.7</v>
       </c>
       <c r="I10">
-        <v>53.743254299999997</v>
+        <v>51.79</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
@@ -863,10 +863,10 @@
         <v>0.5</v>
       </c>
       <c r="H11">
-        <v>-2.7417929999999999</v>
+        <v>-2.4</v>
       </c>
       <c r="I11">
-        <v>54.047049000000001</v>
+        <v>51.71</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
@@ -892,10 +892,10 @@
         <v>0.5</v>
       </c>
       <c r="H12">
-        <v>1.3441399999999999</v>
+        <v>0.35</v>
       </c>
       <c r="I12">
-        <v>51.311549999999997</v>
+        <v>52.22</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
@@ -921,10 +921,10 @@
         <v>0.5</v>
       </c>
       <c r="H13">
-        <v>-2.3588399999999998</v>
+        <v>0.87</v>
       </c>
       <c r="I13">
-        <v>53.539050000000003</v>
+        <v>52.980000000000004</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.45">
@@ -950,10 +950,10 @@
         <v>0.5</v>
       </c>
       <c r="H14">
-        <v>-2.8412730000000002</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="I14">
-        <v>51.339275999999998</v>
+        <v>52.56</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.45">
@@ -979,10 +979,10 @@
         <v>0.5</v>
       </c>
       <c r="H15">
-        <v>-1.2377826000000001</v>
+        <v>-1.62</v>
       </c>
       <c r="I15">
-        <v>53.6055098</v>
+        <v>52.56</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.45">
@@ -1008,10 +1008,10 @@
         <v>0.5</v>
       </c>
       <c r="H16">
-        <v>-1.2668429000000001</v>
+        <v>-1.88</v>
       </c>
       <c r="I16">
-        <v>53.7563338</v>
+        <v>52.13</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
@@ -1037,10 +1037,10 @@
         <v>0.5</v>
       </c>
       <c r="H17">
-        <v>-1.8523677000000001</v>
+        <v>-2.8</v>
       </c>
       <c r="I17">
-        <v>52.506843000000003</v>
+        <v>52.980000000000004</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
@@ -1066,10 +1066,10 @@
         <v>0.5</v>
       </c>
       <c r="H18">
-        <v>-1.4579907999999999</v>
+        <v>-1.88</v>
       </c>
       <c r="I18">
-        <v>54.880797999999999</v>
+        <v>52.980000000000004</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
@@ -1095,10 +1095,10 @@
         <v>0.5</v>
       </c>
       <c r="H19">
-        <v>-2.0230397999999998</v>
+        <v>-0.83</v>
       </c>
       <c r="I19">
-        <v>52.499436299999999</v>
+        <v>52.9</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.45">
@@ -1124,10 +1124,10 @@
         <v>0.5</v>
       </c>
       <c r="H20">
-        <v>-1.598063</v>
+        <v>-4.5</v>
       </c>
       <c r="I20">
-        <v>53.806248699999998</v>
+        <v>53.07</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -1153,10 +1153,10 @@
         <v>0.5</v>
       </c>
       <c r="H21">
-        <v>-1.1317391999999999</v>
+        <v>-3.06</v>
       </c>
       <c r="I21">
-        <v>54.566970599999998</v>
+        <v>53.660000000000004</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
@@ -1182,10 +1182,10 @@
         <v>0.5</v>
       </c>
       <c r="H22">
-        <v>-0.49886560000000002</v>
+        <v>-2.3588399999999998</v>
       </c>
       <c r="I22">
-        <v>51.544126499999997</v>
+        <v>53.539050000000003</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -1211,10 +1211,10 @@
         <v>0.5</v>
       </c>
       <c r="H23">
-        <v>-0.75620799999999999</v>
+        <v>-1.49</v>
       </c>
       <c r="I23">
-        <v>53.598061899999998</v>
+        <v>53.57</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.45">
@@ -1240,10 +1240,10 @@
         <v>0.5</v>
       </c>
       <c r="H24">
-        <v>-0.2961377</v>
+        <v>-0.31</v>
       </c>
       <c r="I24">
-        <v>51.501852999999997</v>
+        <v>53.57</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.45">
@@ -1269,10 +1269,10 @@
         <v>0.5</v>
       </c>
       <c r="H25">
-        <v>-0.30164459999999998</v>
+        <v>-0.96</v>
       </c>
       <c r="I25">
-        <v>53.214646999999999</v>
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.45">
@@ -1298,10 +1298,10 @@
         <v>0.5</v>
       </c>
       <c r="H26">
-        <v>-0.2384869</v>
+        <v>-2.0099999999999998</v>
       </c>
       <c r="I26">
-        <v>53.638412099999996</v>
+        <v>54.08</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.45">
@@ -1327,10 +1327,10 @@
         <v>0.5</v>
       </c>
       <c r="H27">
-        <v>0.15460160000000001</v>
+        <v>-2.67</v>
       </c>
       <c r="I27">
-        <v>51.432685800000002</v>
+        <v>54.85</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.45">
@@ -1356,10 +1356,10 @@
         <v>0.5</v>
       </c>
       <c r="H28">
-        <v>-1.2320606999999999</v>
+        <v>-1.23</v>
       </c>
       <c r="I28">
-        <v>50.884506600000002</v>
+        <v>55.1</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.45">
@@ -1385,10 +1385,10 @@
         <v>0.5</v>
       </c>
       <c r="H29">
-        <v>0.31190000000000001</v>
+        <v>-0.44</v>
       </c>
       <c r="I29">
-        <v>51.490805000000002</v>
+        <v>54.76</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.45">
@@ -1414,14 +1414,15 @@
         <v>0.5</v>
       </c>
       <c r="H30">
-        <v>0.50670380000000004</v>
+        <v>0.21</v>
       </c>
       <c r="I30">
-        <v>51.512869000000002</v>
+        <v>54.08</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1429,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1720D-7D07-42E6-8F89-C1A31D3BEF41}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
1) Added 'combine_extracted_scenarios' in scenario_generation_model.py. Now we can:  1# generate a number of single scenarios using the existing function 'generate_ws_scenario', 2# select effective windstorm scenarios from the generated candidate single scenarios, 3# extract the windstorm window of these selected scenarios using 'extract_ws_scenarios', 4# combine the extracted scenarios into a single .json file that can be used for the investment model using 'combine_extracted_scenarios'. The process from 1# to 4# has been coded in a separate script 'select_and_combine_ws_scenarios.py'
</commit_message>
<xml_diff>
--- a/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
+++ b/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\GB_Network_29bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E563BCCC-1FEA-4632-ACBC-A1F375E8AE94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F58723A-0D73-4121-97EF-293CCD09AB8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F290B48-A8E1-43D7-A531-2D8691AE6FE2}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
1) Modified the network modelling of the 29-bus GB transmission network: Now added a few grid interconnection point, modelled as virtual generators at the corresponding buses with -5000~5000 generation capacity and (0, 50) generation cost model, through modifying the data input file 'GB_Transmission_Network_29_Bus.xlsx'.
2) Improved scripts 'visualize_pareto_fronts.py', and created a visualization script 'visualize_network_topology.py'.

3) Created a script 'extract_optimisation_results_from_excel.py' (contents imported from the previous test_2.py)
</commit_message>
<xml_diff>
--- a/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
+++ b/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\GB_Network_29bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A0BD58-AE02-419D-A08A-0A1CEC639D0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD477ABA-9AE6-41E0-8FB5-F85F3133833E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="-18790" windowWidth="28800" windowHeight="15290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base_values" sheetId="1" r:id="rId1"/>
@@ -537,8 +537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F290B48-A8E1-43D7-A531-2D8691AE6FE2}">
   <dimension ref="A1:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1430,7 +1430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C1720D-7D07-42E6-8F89-C1A31D3BEF41}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
@@ -5875,10 +5875,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B76F648-0BE9-4818-BE21-E619EBC34941}">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K76" sqref="K76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7409,6 +7409,121 @@
         <v>53.661538461538463</v>
       </c>
     </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A67">
+        <v>5</v>
+      </c>
+      <c r="C67">
+        <v>5000</v>
+      </c>
+      <c r="D67">
+        <v>-5000</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A68">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>5000</v>
+      </c>
+      <c r="D68">
+        <v>-5000</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A69">
+        <v>11</v>
+      </c>
+      <c r="C69">
+        <v>5000</v>
+      </c>
+      <c r="D69">
+        <v>-5000</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A70">
+        <v>26</v>
+      </c>
+      <c r="C70">
+        <v>5000</v>
+      </c>
+      <c r="D70">
+        <v>-5000</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
+      <c r="H70">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A71">
+        <v>27</v>
+      </c>
+      <c r="C71">
+        <v>5000</v>
+      </c>
+      <c r="D71">
+        <v>-5000</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
1) (Important) Added a new scenario generation script based on MCS with convergence criterion: ws_scenario_library_generator_with_convergence.py.
2) Debugged and improved the method 'build_combined_opf_model_under_ws_scenarios' in network.py.

3) Updated the Kearsley_GSP_group_only_modified.xlsx. --> Now there's no EENS across the 1-year period in the normal-operation scenario.

4) Updated GB_Transmission_Network_29_Bus.xlsx. --> Now each grid interconnection is modelled as two separate generators (with positive import cost but zero export cost).

5) Minor changes across the project.
</commit_message>
<xml_diff>
--- a/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
+++ b/Input_Data/GB_Network_29bus/GB_Transmission_Network_29_Bus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Documents_Unsynced\Python_Projects\Investment_Planning_Model\investment_planning_model\Input_Data\GB_Network_29bus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD477ABA-9AE6-41E0-8FB5-F85F3133833E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC0F7C11-D68D-4E52-A3D5-F35587F8AE40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-21720" windowWidth="38640" windowHeight="21120" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -157,6 +157,9 @@
   </si>
   <si>
     <t>If Hardenable</t>
+  </si>
+  <si>
+    <t>interconnector</t>
   </si>
 </sst>
 </file>
@@ -5875,10 +5878,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B76F648-0BE9-4818-BE21-E619EBC34941}">
-  <dimension ref="A1:H71"/>
+  <dimension ref="A1:H76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K76" sqref="K76"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7413,11 +7416,14 @@
       <c r="A67">
         <v>5</v>
       </c>
+      <c r="B67" t="s">
+        <v>39</v>
+      </c>
       <c r="C67">
         <v>5000</v>
       </c>
       <c r="D67">
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="E67">
         <v>0</v>
@@ -7434,10 +7440,13 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A68">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="B68" t="s">
+        <v>39</v>
       </c>
       <c r="C68">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D68">
         <v>-5000</v>
@@ -7452,18 +7461,21 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A69">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B69" t="s">
+        <v>39</v>
       </c>
       <c r="C69">
         <v>5000</v>
       </c>
       <c r="D69">
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -7480,10 +7492,13 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A70">
-        <v>26</v>
+        <v>10</v>
+      </c>
+      <c r="B70" t="s">
+        <v>39</v>
       </c>
       <c r="C70">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="D70">
         <v>-5000</v>
@@ -7498,18 +7513,21 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>50</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A71">
-        <v>27</v>
+        <v>11</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
       </c>
       <c r="C71">
         <v>5000</v>
       </c>
       <c r="D71">
-        <v>-5000</v>
+        <v>0</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -7522,6 +7540,136 @@
       </c>
       <c r="H71">
         <v>50</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A72">
+        <v>11</v>
+      </c>
+      <c r="B72" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>-5000</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A73">
+        <v>26</v>
+      </c>
+      <c r="B73" t="s">
+        <v>39</v>
+      </c>
+      <c r="C73">
+        <v>5000</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A74">
+        <v>26</v>
+      </c>
+      <c r="B74" t="s">
+        <v>39</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>-5000</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A75">
+        <v>27</v>
+      </c>
+      <c r="B75" t="s">
+        <v>39</v>
+      </c>
+      <c r="C75">
+        <v>5000</v>
+      </c>
+      <c r="D75">
+        <v>0</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A76">
+        <v>27</v>
+      </c>
+      <c r="B76" t="s">
+        <v>39</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>-5000</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>